<commit_message>
Added pie chart with put/call freq.
</commit_message>
<xml_diff>
--- a/OptionTrades.xlsx
+++ b/OptionTrades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="457">
   <si>
     <t>Option Name</t>
   </si>
@@ -832,553 +832,559 @@
     <t>AAPL $380.0000 call 2020-07-10</t>
   </si>
   <si>
-    <t>289.0000</t>
-  </si>
-  <si>
-    <t>540.0000</t>
-  </si>
-  <si>
-    <t>188.0000</t>
-  </si>
-  <si>
-    <t>171.3333</t>
-  </si>
-  <si>
-    <t>100.5556</t>
-  </si>
-  <si>
-    <t>432.5000</t>
-  </si>
-  <si>
-    <t>130.0000</t>
-  </si>
-  <si>
-    <t>184.0000</t>
-  </si>
-  <si>
-    <t>1890.0000</t>
-  </si>
-  <si>
-    <t>1025.0000</t>
-  </si>
-  <si>
-    <t>987.5000</t>
-  </si>
-  <si>
-    <t>372.0000</t>
-  </si>
-  <si>
-    <t>1600.0000</t>
-  </si>
-  <si>
-    <t>207.0000</t>
-  </si>
-  <si>
-    <t>535.0000</t>
-  </si>
-  <si>
-    <t>232.6667</t>
-  </si>
-  <si>
-    <t>1190.0000</t>
-  </si>
-  <si>
-    <t>39.0000</t>
-  </si>
-  <si>
-    <t>335.7500</t>
-  </si>
-  <si>
-    <t>191.0000</t>
-  </si>
-  <si>
-    <t>165.0000</t>
-  </si>
-  <si>
-    <t>425.0000</t>
-  </si>
-  <si>
-    <t>205.6667</t>
-  </si>
-  <si>
-    <t>430.0000</t>
-  </si>
-  <si>
-    <t>296.6667</t>
-  </si>
-  <si>
-    <t>1405.0000</t>
-  </si>
-  <si>
-    <t>42.0000</t>
-  </si>
-  <si>
-    <t>0.0000</t>
-  </si>
-  <si>
-    <t>154.0000</t>
-  </si>
-  <si>
-    <t>356.0000</t>
-  </si>
-  <si>
-    <t>450.0000</t>
-  </si>
-  <si>
-    <t>480.0000</t>
-  </si>
-  <si>
-    <t>10.0000</t>
-  </si>
-  <si>
-    <t>297.0000</t>
-  </si>
-  <si>
-    <t>158.0000</t>
-  </si>
-  <si>
-    <t>204.2500</t>
-  </si>
-  <si>
-    <t>299.0000</t>
-  </si>
-  <si>
-    <t>472.5000</t>
-  </si>
-  <si>
-    <t>381.6667</t>
-  </si>
-  <si>
-    <t>520.0000</t>
-  </si>
-  <si>
-    <t>90.0000</t>
-  </si>
-  <si>
-    <t>1100.0000</t>
-  </si>
-  <si>
-    <t>320.0000</t>
-  </si>
-  <si>
-    <t>400.0000</t>
-  </si>
-  <si>
-    <t>1455.0000</t>
-  </si>
-  <si>
-    <t>167.0000</t>
-  </si>
-  <si>
-    <t>775.0000</t>
-  </si>
-  <si>
-    <t>955.0000</t>
-  </si>
-  <si>
-    <t>215.0000</t>
-  </si>
-  <si>
-    <t>310.0000</t>
-  </si>
-  <si>
-    <t>296.0000</t>
-  </si>
-  <si>
-    <t>995.0000</t>
-  </si>
-  <si>
-    <t>858.3333</t>
-  </si>
-  <si>
-    <t>258.0000</t>
-  </si>
-  <si>
-    <t>692.5000</t>
-  </si>
-  <si>
-    <t>542.5000</t>
-  </si>
-  <si>
-    <t>239.0000</t>
-  </si>
-  <si>
-    <t>316.5000</t>
-  </si>
-  <si>
-    <t>128.5000</t>
-  </si>
-  <si>
-    <t>365.5000</t>
-  </si>
-  <si>
-    <t>283.0000</t>
-  </si>
-  <si>
-    <t>409.0000</t>
-  </si>
-  <si>
-    <t>396.0000</t>
-  </si>
-  <si>
-    <t>449.0000</t>
-  </si>
-  <si>
-    <t>1277.5000</t>
-  </si>
-  <si>
-    <t>1500.0000</t>
-  </si>
-  <si>
-    <t>459.0000</t>
-  </si>
-  <si>
-    <t>1165.0000</t>
-  </si>
-  <si>
-    <t>470.0000</t>
-  </si>
-  <si>
-    <t>770.0000</t>
-  </si>
-  <si>
-    <t>230.0000</t>
-  </si>
-  <si>
-    <t>511.2500</t>
-  </si>
-  <si>
-    <t>1685.0000</t>
-  </si>
-  <si>
-    <t>26.3333</t>
-  </si>
-  <si>
-    <t>270.0000</t>
-  </si>
-  <si>
-    <t>77.7500</t>
-  </si>
-  <si>
-    <t>557.5000</t>
-  </si>
-  <si>
-    <t>387.5000</t>
-  </si>
-  <si>
-    <t>144.0000</t>
-  </si>
-  <si>
-    <t>147.7143</t>
-  </si>
-  <si>
-    <t>56.8000</t>
-  </si>
-  <si>
-    <t>307.5000</t>
-  </si>
-  <si>
-    <t>226.0000</t>
-  </si>
-  <si>
-    <t>330.0000</t>
-  </si>
-  <si>
-    <t>315.0000</t>
-  </si>
-  <si>
-    <t>385.0000</t>
-  </si>
-  <si>
-    <t>177.0000</t>
-  </si>
-  <si>
-    <t>38.0000</t>
-  </si>
-  <si>
-    <t>75.0000</t>
-  </si>
-  <si>
-    <t>275.0000</t>
-  </si>
-  <si>
-    <t>241.0000</t>
-  </si>
-  <si>
-    <t>145.0000</t>
-  </si>
-  <si>
-    <t>187.0000</t>
-  </si>
-  <si>
-    <t>181.3333</t>
-  </si>
-  <si>
-    <t>193.0000</t>
-  </si>
-  <si>
-    <t>267.0834</t>
-  </si>
-  <si>
-    <t>870.0000</t>
-  </si>
-  <si>
-    <t>120.0000</t>
-  </si>
-  <si>
-    <t>80.7143</t>
-  </si>
-  <si>
-    <t>575.0000</t>
-  </si>
-  <si>
-    <t>275.7428</t>
-  </si>
-  <si>
-    <t>305.0000</t>
-  </si>
-  <si>
-    <t>311.0000</t>
-  </si>
-  <si>
-    <t>1155.0000</t>
-  </si>
-  <si>
-    <t>860.0000</t>
-  </si>
-  <si>
-    <t>180.0000</t>
-  </si>
-  <si>
-    <t>280.0000</t>
-  </si>
-  <si>
-    <t>625.0000</t>
-  </si>
-  <si>
-    <t>293.0000</t>
-  </si>
-  <si>
-    <t>391.0000</t>
-  </si>
-  <si>
-    <t>135.0000</t>
-  </si>
-  <si>
-    <t>109.0000</t>
-  </si>
-  <si>
-    <t>689.0000</t>
-  </si>
-  <si>
-    <t>835.0000</t>
-  </si>
-  <si>
-    <t>202.5000</t>
-  </si>
-  <si>
-    <t>157.5714</t>
-  </si>
-  <si>
-    <t>325.0000</t>
-  </si>
-  <si>
-    <t>350.0000</t>
-  </si>
-  <si>
-    <t>266.0000</t>
-  </si>
-  <si>
-    <t>286.7500</t>
-  </si>
-  <si>
-    <t>555.0000</t>
-  </si>
-  <si>
-    <t>150.0000</t>
-  </si>
-  <si>
-    <t>192.0000</t>
-  </si>
-  <si>
-    <t>530.0000</t>
-  </si>
-  <si>
-    <t>620.0000</t>
-  </si>
-  <si>
-    <t>222.0000</t>
-  </si>
-  <si>
-    <t>550.0000</t>
-  </si>
-  <si>
-    <t>492.0000</t>
-  </si>
-  <si>
-    <t>77.0000</t>
-  </si>
-  <si>
-    <t>757.5000</t>
-  </si>
-  <si>
-    <t>289.5000</t>
-  </si>
-  <si>
-    <t>700.0000</t>
-  </si>
-  <si>
-    <t>103.5000</t>
-  </si>
-  <si>
-    <t>362.2500</t>
-  </si>
-  <si>
-    <t>139.0000</t>
-  </si>
-  <si>
-    <t>112.0000</t>
-  </si>
-  <si>
-    <t>124.0000</t>
-  </si>
-  <si>
-    <t>271.0000</t>
-  </si>
-  <si>
-    <t>352.0000</t>
-  </si>
-  <si>
-    <t>1315.0000</t>
-  </si>
-  <si>
-    <t>705.0000</t>
-  </si>
-  <si>
-    <t>695.0000</t>
-  </si>
-  <si>
-    <t>571.2500</t>
-  </si>
-  <si>
-    <t>887.5000</t>
-  </si>
-  <si>
-    <t>1780.0000</t>
-  </si>
-  <si>
-    <t>2525.0000</t>
-  </si>
-  <si>
-    <t>737.5000</t>
-  </si>
-  <si>
-    <t>48.0000</t>
-  </si>
-  <si>
-    <t>420.0000</t>
-  </si>
-  <si>
-    <t>50.0000</t>
-  </si>
-  <si>
-    <t>207.5000</t>
-  </si>
-  <si>
-    <t>57.2500</t>
-  </si>
-  <si>
-    <t>655.0000</t>
-  </si>
-  <si>
-    <t>577.5000</t>
-  </si>
-  <si>
-    <t>1665.0000</t>
-  </si>
-  <si>
-    <t>670.0000</t>
-  </si>
-  <si>
-    <t>565.0000</t>
-  </si>
-  <si>
-    <t>1240.0000</t>
-  </si>
-  <si>
-    <t>755.0000</t>
-  </si>
-  <si>
-    <t>85.0000</t>
-  </si>
-  <si>
-    <t>1270.0000</t>
-  </si>
-  <si>
-    <t>110.0000</t>
-  </si>
-  <si>
-    <t>44.0000</t>
-  </si>
-  <si>
-    <t>47.0000</t>
-  </si>
-  <si>
-    <t>261.0000</t>
-  </si>
-  <si>
-    <t>505.0000</t>
-  </si>
-  <si>
-    <t>146.0000</t>
-  </si>
-  <si>
-    <t>64.0000</t>
-  </si>
-  <si>
-    <t>460.0000</t>
-  </si>
-  <si>
-    <t>455.0000</t>
-  </si>
-  <si>
-    <t>380.0000</t>
-  </si>
-  <si>
-    <t>645.0000</t>
-  </si>
-  <si>
-    <t>182.0000</t>
-  </si>
-  <si>
-    <t>980.0000</t>
-  </si>
-  <si>
-    <t>317.5000</t>
-  </si>
-  <si>
-    <t>138.0000</t>
-  </si>
-  <si>
-    <t>68.0000</t>
-  </si>
-  <si>
-    <t>226.2500</t>
-  </si>
-  <si>
-    <t>100.0000</t>
-  </si>
-  <si>
-    <t>351.6667</t>
-  </si>
-  <si>
-    <t>98.0000</t>
-  </si>
-  <si>
-    <t>170.0000</t>
-  </si>
-  <si>
-    <t>610.0000</t>
+    <t>$289.0000</t>
+  </si>
+  <si>
+    <t>$540.0000</t>
+  </si>
+  <si>
+    <t>$188.0000</t>
+  </si>
+  <si>
+    <t>$171.3333</t>
+  </si>
+  <si>
+    <t>$100.5556</t>
+  </si>
+  <si>
+    <t>$432.5000</t>
+  </si>
+  <si>
+    <t>$130.0000</t>
+  </si>
+  <si>
+    <t>$184.0000</t>
+  </si>
+  <si>
+    <t>$1890.0000</t>
+  </si>
+  <si>
+    <t>$1025.0000</t>
+  </si>
+  <si>
+    <t>$987.5000</t>
+  </si>
+  <si>
+    <t>$372.0000</t>
+  </si>
+  <si>
+    <t>$1600.0000</t>
+  </si>
+  <si>
+    <t>$207.0000</t>
+  </si>
+  <si>
+    <t>$535.0000</t>
+  </si>
+  <si>
+    <t>$232.6667</t>
+  </si>
+  <si>
+    <t>$1190.0000</t>
+  </si>
+  <si>
+    <t>$39.0000</t>
+  </si>
+  <si>
+    <t>$335.7500</t>
+  </si>
+  <si>
+    <t>$191.0000</t>
+  </si>
+  <si>
+    <t>$165.0000</t>
+  </si>
+  <si>
+    <t>$425.0000</t>
+  </si>
+  <si>
+    <t>$205.6667</t>
+  </si>
+  <si>
+    <t>$430.0000</t>
+  </si>
+  <si>
+    <t>$296.6667</t>
+  </si>
+  <si>
+    <t>$1405.0000</t>
+  </si>
+  <si>
+    <t>$42.0000</t>
+  </si>
+  <si>
+    <t>$0.0000</t>
+  </si>
+  <si>
+    <t>$154.0000</t>
+  </si>
+  <si>
+    <t>$356.0000</t>
+  </si>
+  <si>
+    <t>$450.0000</t>
+  </si>
+  <si>
+    <t>$480.0000</t>
+  </si>
+  <si>
+    <t>$10.0000</t>
+  </si>
+  <si>
+    <t>$297.0000</t>
+  </si>
+  <si>
+    <t>$158.0000</t>
+  </si>
+  <si>
+    <t>$204.2500</t>
+  </si>
+  <si>
+    <t>$299.0000</t>
+  </si>
+  <si>
+    <t>$472.5000</t>
+  </si>
+  <si>
+    <t>$381.6667</t>
+  </si>
+  <si>
+    <t>$520.0000</t>
+  </si>
+  <si>
+    <t>$90.0000</t>
+  </si>
+  <si>
+    <t>$1100.0000</t>
+  </si>
+  <si>
+    <t>$320.0000</t>
+  </si>
+  <si>
+    <t>$400.0000</t>
+  </si>
+  <si>
+    <t>$1455.0000</t>
+  </si>
+  <si>
+    <t>$167.0000</t>
+  </si>
+  <si>
+    <t>$775.0000</t>
+  </si>
+  <si>
+    <t>$955.0000</t>
+  </si>
+  <si>
+    <t>$215.0000</t>
+  </si>
+  <si>
+    <t>$310.0000</t>
+  </si>
+  <si>
+    <t>$296.0000</t>
+  </si>
+  <si>
+    <t>$995.0000</t>
+  </si>
+  <si>
+    <t>$858.3333</t>
+  </si>
+  <si>
+    <t>$258.0000</t>
+  </si>
+  <si>
+    <t>$692.5000</t>
+  </si>
+  <si>
+    <t>$542.5000</t>
+  </si>
+  <si>
+    <t>$239.0000</t>
+  </si>
+  <si>
+    <t>$316.5000</t>
+  </si>
+  <si>
+    <t>$128.5000</t>
+  </si>
+  <si>
+    <t>$365.5000</t>
+  </si>
+  <si>
+    <t>$283.0000</t>
+  </si>
+  <si>
+    <t>$409.0000</t>
+  </si>
+  <si>
+    <t>$396.0000</t>
+  </si>
+  <si>
+    <t>$449.0000</t>
+  </si>
+  <si>
+    <t>$1277.5000</t>
+  </si>
+  <si>
+    <t>$1500.0000</t>
+  </si>
+  <si>
+    <t>$459.0000</t>
+  </si>
+  <si>
+    <t>$1165.0000</t>
+  </si>
+  <si>
+    <t>$470.0000</t>
+  </si>
+  <si>
+    <t>$770.0000</t>
+  </si>
+  <si>
+    <t>$230.0000</t>
+  </si>
+  <si>
+    <t>$511.2500</t>
+  </si>
+  <si>
+    <t>$1685.0000</t>
+  </si>
+  <si>
+    <t>$26.3333</t>
+  </si>
+  <si>
+    <t>$270.0000</t>
+  </si>
+  <si>
+    <t>$77.7500</t>
+  </si>
+  <si>
+    <t>$557.5000</t>
+  </si>
+  <si>
+    <t>$387.5000</t>
+  </si>
+  <si>
+    <t>$144.0000</t>
+  </si>
+  <si>
+    <t>$147.7143</t>
+  </si>
+  <si>
+    <t>$56.8000</t>
+  </si>
+  <si>
+    <t>$307.5000</t>
+  </si>
+  <si>
+    <t>$226.0000</t>
+  </si>
+  <si>
+    <t>$330.0000</t>
+  </si>
+  <si>
+    <t>$315.0000</t>
+  </si>
+  <si>
+    <t>$385.0000</t>
+  </si>
+  <si>
+    <t>$177.0000</t>
+  </si>
+  <si>
+    <t>$38.0000</t>
+  </si>
+  <si>
+    <t>$75.0000</t>
+  </si>
+  <si>
+    <t>$275.0000</t>
+  </si>
+  <si>
+    <t>$241.0000</t>
+  </si>
+  <si>
+    <t>$145.0000</t>
+  </si>
+  <si>
+    <t>$187.0000</t>
+  </si>
+  <si>
+    <t>$181.3333</t>
+  </si>
+  <si>
+    <t>$193.0000</t>
+  </si>
+  <si>
+    <t>$267.0834</t>
+  </si>
+  <si>
+    <t>$870.0000</t>
+  </si>
+  <si>
+    <t>$120.0000</t>
+  </si>
+  <si>
+    <t>$80.7143</t>
+  </si>
+  <si>
+    <t>$575.0000</t>
+  </si>
+  <si>
+    <t>$275.7428</t>
+  </si>
+  <si>
+    <t>$305.0000</t>
+  </si>
+  <si>
+    <t>$311.0000</t>
+  </si>
+  <si>
+    <t>$1155.0000</t>
+  </si>
+  <si>
+    <t>$860.0000</t>
+  </si>
+  <si>
+    <t>$180.0000</t>
+  </si>
+  <si>
+    <t>$280.0000</t>
+  </si>
+  <si>
+    <t>$625.0000</t>
+  </si>
+  <si>
+    <t>$293.0000</t>
+  </si>
+  <si>
+    <t>$391.0000</t>
+  </si>
+  <si>
+    <t>$135.0000</t>
+  </si>
+  <si>
+    <t>$109.0000</t>
+  </si>
+  <si>
+    <t>$689.0000</t>
+  </si>
+  <si>
+    <t>$835.0000</t>
+  </si>
+  <si>
+    <t>$202.5000</t>
+  </si>
+  <si>
+    <t>$157.5714</t>
+  </si>
+  <si>
+    <t>$325.0000</t>
+  </si>
+  <si>
+    <t>$350.0000</t>
+  </si>
+  <si>
+    <t>$266.0000</t>
+  </si>
+  <si>
+    <t>$286.7500</t>
+  </si>
+  <si>
+    <t>$555.0000</t>
+  </si>
+  <si>
+    <t>$150.0000</t>
+  </si>
+  <si>
+    <t>$192.0000</t>
+  </si>
+  <si>
+    <t>$530.0000</t>
+  </si>
+  <si>
+    <t>$620.0000</t>
+  </si>
+  <si>
+    <t>$222.0000</t>
+  </si>
+  <si>
+    <t>$550.0000</t>
+  </si>
+  <si>
+    <t>$492.0000</t>
+  </si>
+  <si>
+    <t>$77.0000</t>
+  </si>
+  <si>
+    <t>$757.5000</t>
+  </si>
+  <si>
+    <t>$289.5000</t>
+  </si>
+  <si>
+    <t>$700.0000</t>
+  </si>
+  <si>
+    <t>$103.5000</t>
+  </si>
+  <si>
+    <t>$362.2500</t>
+  </si>
+  <si>
+    <t>$139.0000</t>
+  </si>
+  <si>
+    <t>$112.0000</t>
+  </si>
+  <si>
+    <t>$124.0000</t>
+  </si>
+  <si>
+    <t>$271.0000</t>
+  </si>
+  <si>
+    <t>$352.0000</t>
+  </si>
+  <si>
+    <t>$1315.0000</t>
+  </si>
+  <si>
+    <t>$705.0000</t>
+  </si>
+  <si>
+    <t>$695.0000</t>
+  </si>
+  <si>
+    <t>$571.2500</t>
+  </si>
+  <si>
+    <t>$887.5000</t>
+  </si>
+  <si>
+    <t>$1780.0000</t>
+  </si>
+  <si>
+    <t>$2525.0000</t>
+  </si>
+  <si>
+    <t>$737.5000</t>
+  </si>
+  <si>
+    <t>$48.0000</t>
+  </si>
+  <si>
+    <t>$420.0000</t>
+  </si>
+  <si>
+    <t>$50.0000</t>
+  </si>
+  <si>
+    <t>$207.5000</t>
+  </si>
+  <si>
+    <t>$57.2500</t>
+  </si>
+  <si>
+    <t>$655.0000</t>
+  </si>
+  <si>
+    <t>$577.5000</t>
+  </si>
+  <si>
+    <t>$1665.0000</t>
+  </si>
+  <si>
+    <t>$670.0000</t>
+  </si>
+  <si>
+    <t>$565.0000</t>
+  </si>
+  <si>
+    <t>$1240.0000</t>
+  </si>
+  <si>
+    <t>$755.0000</t>
+  </si>
+  <si>
+    <t>$85.0000</t>
+  </si>
+  <si>
+    <t>$1270.0000</t>
+  </si>
+  <si>
+    <t>$110.0000</t>
+  </si>
+  <si>
+    <t>$44.0000</t>
+  </si>
+  <si>
+    <t>$47.0000</t>
+  </si>
+  <si>
+    <t>$261.0000</t>
+  </si>
+  <si>
+    <t>$505.0000</t>
+  </si>
+  <si>
+    <t>$146.0000</t>
+  </si>
+  <si>
+    <t>$64.0000</t>
+  </si>
+  <si>
+    <t>$460.0000</t>
+  </si>
+  <si>
+    <t>$455.0000</t>
+  </si>
+  <si>
+    <t>$380.0000</t>
+  </si>
+  <si>
+    <t>$645.0000</t>
+  </si>
+  <si>
+    <t>$182.0000</t>
+  </si>
+  <si>
+    <t>$980.0000</t>
+  </si>
+  <si>
+    <t>$317.5000</t>
+  </si>
+  <si>
+    <t>$138.0000</t>
+  </si>
+  <si>
+    <t>$68.0000</t>
+  </si>
+  <si>
+    <t>$226.2500</t>
+  </si>
+  <si>
+    <t>$100.0000</t>
+  </si>
+  <si>
+    <t>$351.6667</t>
+  </si>
+  <si>
+    <t>$98.0000</t>
+  </si>
+  <si>
+    <t>$170.0000</t>
+  </si>
+  <si>
+    <t>$610.0000</t>
+  </si>
+  <si>
+    <t>Calls</t>
+  </si>
+  <si>
+    <t>Puts</t>
   </si>
 </sst>
 </file>
@@ -1449,6 +1455,135 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="10"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Call vs Put Frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Pie sales data</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Calls</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Puts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1736,13 +1871,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C271"/>
+  <dimension ref="A1:F271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1750,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1760,8 +1895,14 @@
       <c r="C2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" t="s">
+        <v>455</v>
+      </c>
+      <c r="F2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1771,8 +1912,14 @@
       <c r="C3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <v>197</v>
+      </c>
+      <c r="F3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1783,7 +1930,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1794,7 +1941,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1805,7 +1952,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1816,7 +1963,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1827,7 +1974,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1838,7 +1985,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1849,7 +1996,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1860,7 +2007,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1871,7 +2018,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1882,7 +2029,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1893,7 +2040,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1904,7 +2051,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4722,5 +4869,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added ticker frequency list - fix chart.
</commit_message>
<xml_diff>
--- a/OptionTrades.xlsx
+++ b/OptionTrades.xlsx
@@ -7,14 +7,50 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Options" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="469">
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>SPY</t>
+  </si>
+  <si>
+    <t>QQQ</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>CHWY</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>FSLY</t>
+  </si>
+  <si>
+    <t>VXX</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
   <si>
     <t>Option Name</t>
   </si>
@@ -1491,12 +1527,12 @@
             <c:v>Pie sales data</c:v>
           </c:tx>
           <c:dLbls>
-            <c:showVal val="1"/>
             <c:showCatName val="1"/>
+            <c:showPercent val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$2:$F$2</c:f>
+              <c:f>Options!$F$2:$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1510,7 +1546,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$F$3</c:f>
+              <c:f>Options!$F$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1551,20 +1587,105 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="10"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ticker Frequency</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ticker Frequency</c:v>
+          </c:tx>
+          <c:dLbls>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Options!$N$4:$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="1">
+                  <c:v>Ticker</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Options!$N$5:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="0"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1578,6 +1699,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1871,195 +2022,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F271"/>
+  <dimension ref="A1:P271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E2" t="s">
-        <v>455</v>
-      </c>
-      <c r="F2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>284</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E3">
+        <v>285</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>197</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>286</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>287</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>288</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>289</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>290</v>
+      </c>
+      <c r="N8" s="1">
+        <v>3</v>
+      </c>
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>291</v>
+      </c>
+      <c r="N9" s="1">
+        <v>4</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>292</v>
+      </c>
+      <c r="N10" s="1">
+        <v>5</v>
+      </c>
+      <c r="O10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>293</v>
+      </c>
+      <c r="N11" s="1">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>294</v>
+      </c>
+      <c r="N12" s="1">
+        <v>7</v>
+      </c>
+      <c r="O12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>295</v>
+      </c>
+      <c r="N13" s="1">
+        <v>8</v>
+      </c>
+      <c r="O13" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>291</v>
+      </c>
+      <c r="N14" s="1">
+        <v>9</v>
+      </c>
+      <c r="O14" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2067,10 +2317,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2078,10 +2328,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2089,10 +2339,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2100,10 +2350,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2111,10 +2361,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2122,10 +2372,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2133,10 +2383,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2144,10 +2394,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2155,10 +2405,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2166,10 +2416,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2177,10 +2427,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2188,10 +2438,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2199,10 +2449,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2210,10 +2460,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2221,10 +2471,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2232,10 +2482,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2243,10 +2493,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2254,10 +2504,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2265,10 +2515,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2276,10 +2526,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2287,10 +2537,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2298,10 +2548,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2309,10 +2559,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2320,10 +2570,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2331,10 +2581,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2342,10 +2592,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2353,10 +2603,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2364,10 +2614,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C44" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2375,10 +2625,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2386,10 +2636,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2397,10 +2647,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2408,10 +2658,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2419,10 +2669,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2430,10 +2680,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2441,10 +2691,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2452,10 +2702,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2463,10 +2713,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2474,10 +2724,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C54" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2485,10 +2735,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2496,10 +2746,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2507,10 +2757,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C57" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2518,10 +2768,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2529,10 +2779,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2540,10 +2790,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2551,10 +2801,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2562,10 +2812,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2573,10 +2823,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2584,10 +2834,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2595,10 +2845,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C65" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2606,10 +2856,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C66" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2617,10 +2867,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C67" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2628,10 +2878,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2639,10 +2889,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C69" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2650,10 +2900,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C70" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2661,10 +2911,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C71" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2672,10 +2922,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2683,10 +2933,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C73" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2694,10 +2944,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C74" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2705,10 +2955,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C75" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2716,10 +2966,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2727,10 +2977,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2738,10 +2988,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C78" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2749,10 +2999,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2760,10 +3010,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C80" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2771,10 +3021,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C81" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2782,10 +3032,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C82" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2793,10 +3043,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2804,10 +3054,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C84" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2815,10 +3065,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C85" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2826,10 +3076,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2837,10 +3087,10 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2848,10 +3098,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C88" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2859,10 +3109,10 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2870,10 +3120,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C90" t="s">
-        <v>353</v>
+        <v>365</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2881,10 +3131,10 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C91" t="s">
-        <v>354</v>
+        <v>366</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2892,10 +3142,10 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C92" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2903,10 +3153,10 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2914,10 +3164,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C94" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2925,10 +3175,10 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C95" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2936,10 +3186,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C96" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2947,10 +3197,10 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C97" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -2958,10 +3208,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C98" t="s">
-        <v>361</v>
+        <v>373</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -2969,10 +3219,10 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C99" t="s">
-        <v>362</v>
+        <v>374</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -2980,10 +3230,10 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C100" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -2991,10 +3241,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C101" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -3002,10 +3252,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C102" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -3013,10 +3263,10 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C103" t="s">
-        <v>366</v>
+        <v>378</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -3024,10 +3274,10 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C104" t="s">
-        <v>367</v>
+        <v>379</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -3035,10 +3285,10 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C105" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -3046,10 +3296,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>368</v>
+        <v>380</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -3057,10 +3307,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
-        <v>369</v>
+        <v>381</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -3068,10 +3318,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C108" t="s">
-        <v>370</v>
+        <v>382</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -3079,10 +3329,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -3090,10 +3340,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
-        <v>372</v>
+        <v>384</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -3101,10 +3351,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C111" t="s">
-        <v>373</v>
+        <v>385</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -3112,10 +3362,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C112" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -3123,10 +3373,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C113" t="s">
-        <v>375</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -3134,10 +3384,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C114" t="s">
-        <v>376</v>
+        <v>388</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -3145,10 +3395,10 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C115" t="s">
-        <v>377</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -3156,10 +3406,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C116" t="s">
-        <v>378</v>
+        <v>390</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -3167,10 +3417,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C117" t="s">
-        <v>379</v>
+        <v>391</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -3178,10 +3428,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C118" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -3189,10 +3439,10 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -3200,10 +3450,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C120" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -3211,10 +3461,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C121" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3222,10 +3472,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C122" t="s">
-        <v>383</v>
+        <v>395</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -3233,10 +3483,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C123" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -3244,10 +3494,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="C124" t="s">
-        <v>384</v>
+        <v>396</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -3255,10 +3505,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C125" t="s">
-        <v>385</v>
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -3266,10 +3516,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="C126" t="s">
-        <v>386</v>
+        <v>398</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -3277,10 +3527,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C127" t="s">
-        <v>387</v>
+        <v>399</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -3288,10 +3538,10 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="C128" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -3299,10 +3549,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C129" t="s">
-        <v>388</v>
+        <v>400</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -3310,10 +3560,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C130" t="s">
-        <v>389</v>
+        <v>401</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -3321,10 +3571,10 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C131" t="s">
-        <v>390</v>
+        <v>402</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -3332,10 +3582,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C132" t="s">
-        <v>391</v>
+        <v>403</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -3343,10 +3593,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="C133" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -3354,10 +3604,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C134" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -3365,10 +3615,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C135" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
     </row>
     <row r="136" spans="1:3">
@@ -3376,10 +3626,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C136" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -3387,10 +3637,10 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C137" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
     </row>
     <row r="138" spans="1:3">
@@ -3398,10 +3648,10 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="C138" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -3409,10 +3659,10 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C139" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -3420,10 +3670,10 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C140" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
     </row>
     <row r="141" spans="1:3">
@@ -3431,10 +3681,10 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C141" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -3442,10 +3692,10 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C142" t="s">
-        <v>400</v>
+        <v>412</v>
       </c>
     </row>
     <row r="143" spans="1:3">
@@ -3453,10 +3703,10 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C143" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -3464,10 +3714,10 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="C144" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
     </row>
     <row r="145" spans="1:3">
@@ -3475,10 +3725,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C145" t="s">
-        <v>403</v>
+        <v>415</v>
       </c>
     </row>
     <row r="146" spans="1:3">
@@ -3486,10 +3736,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C146" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
     </row>
     <row r="147" spans="1:3">
@@ -3497,10 +3747,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C147" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
     </row>
     <row r="148" spans="1:3">
@@ -3508,10 +3758,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="C148" t="s">
-        <v>406</v>
+        <v>418</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -3519,10 +3769,10 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C149" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
     </row>
     <row r="150" spans="1:3">
@@ -3530,10 +3780,10 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="C150" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -3541,10 +3791,10 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="C151" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -3552,10 +3802,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="C152" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -3563,10 +3813,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="C153" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
     </row>
     <row r="154" spans="1:3">
@@ -3574,10 +3824,10 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="C154" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
     </row>
     <row r="155" spans="1:3">
@@ -3585,10 +3835,10 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C155" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -3596,10 +3846,10 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="C156" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -3607,10 +3857,10 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C157" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3618,10 +3868,10 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C158" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -3629,10 +3879,10 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C159" t="s">
-        <v>415</v>
+        <v>427</v>
       </c>
     </row>
     <row r="160" spans="1:3">
@@ -3640,10 +3890,10 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="C160" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -3651,10 +3901,10 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C161" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -3662,10 +3912,10 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="C162" t="s">
-        <v>418</v>
+        <v>430</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -3673,10 +3923,10 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C163" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -3684,10 +3934,10 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C164" t="s">
-        <v>419</v>
+        <v>431</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -3695,10 +3945,10 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="C165" t="s">
-        <v>420</v>
+        <v>432</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -3706,10 +3956,10 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="C166" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3717,10 +3967,10 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="C167" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -3728,10 +3978,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C168" t="s">
-        <v>422</v>
+        <v>434</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -3739,10 +3989,10 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C169" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -3750,10 +4000,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="C170" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -3761,10 +4011,10 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="C171" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -3772,10 +4022,10 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="C172" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -3783,10 +4033,10 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="C173" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
     </row>
     <row r="174" spans="1:3">
@@ -3794,10 +4044,10 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="C174" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3805,10 +4055,10 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="C175" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3816,10 +4066,10 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="C176" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3827,10 +4077,10 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="C177" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3838,10 +4088,10 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C178" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3849,10 +4099,10 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C179" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3860,10 +4110,10 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="C180" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -3871,10 +4121,10 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C181" t="s">
-        <v>412</v>
+        <v>424</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3882,10 +4132,10 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="C182" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3893,10 +4143,10 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="C183" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3904,10 +4154,10 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="C184" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3915,10 +4165,10 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C185" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3926,10 +4176,10 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C186" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3937,10 +4187,10 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C187" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="188" spans="1:3">
@@ -3948,10 +4198,10 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C188" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3959,10 +4209,10 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="C189" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3970,10 +4220,10 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="C190" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3981,10 +4231,10 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C191" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3992,10 +4242,10 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="C192" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -4003,10 +4253,10 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="C193" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -4014,10 +4264,10 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C194" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="195" spans="1:3">
@@ -4025,10 +4275,10 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C195" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
     </row>
     <row r="196" spans="1:3">
@@ -4036,10 +4286,10 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="C196" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -4047,10 +4297,10 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="C197" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -4058,10 +4308,10 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="C198" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
     </row>
     <row r="199" spans="1:3">
@@ -4069,10 +4319,10 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C199" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="200" spans="1:3">
@@ -4080,10 +4330,10 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="C200" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
     </row>
     <row r="201" spans="1:3">
@@ -4091,10 +4341,10 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="C201" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
     </row>
     <row r="202" spans="1:3">
@@ -4102,10 +4352,10 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="C202" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -4113,10 +4363,10 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C203" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -4124,10 +4374,10 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="C204" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -4135,10 +4385,10 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="C205" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -4146,10 +4396,10 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="C206" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -4157,10 +4407,10 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C207" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -4168,10 +4418,10 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="C208" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
     </row>
     <row r="209" spans="1:3">
@@ -4179,10 +4429,10 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="C209" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
     </row>
     <row r="210" spans="1:3">
@@ -4190,10 +4440,10 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C210" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
     </row>
     <row r="211" spans="1:3">
@@ -4201,10 +4451,10 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="C211" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -4212,10 +4462,10 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="C212" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
     </row>
     <row r="213" spans="1:3">
@@ -4223,10 +4473,10 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="C213" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="214" spans="1:3">
@@ -4234,10 +4484,10 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="C214" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -4245,10 +4495,10 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="C215" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -4256,10 +4506,10 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="C216" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="217" spans="1:3">
@@ -4267,10 +4517,10 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C217" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
     </row>
     <row r="218" spans="1:3">
@@ -4278,10 +4528,10 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="C218" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="219" spans="1:3">
@@ -4289,10 +4539,10 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C219" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
     </row>
     <row r="220" spans="1:3">
@@ -4300,10 +4550,10 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="C220" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -4311,10 +4561,10 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="C221" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="222" spans="1:3">
@@ -4322,10 +4572,10 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="C222" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -4333,10 +4583,10 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="C223" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -4344,10 +4594,10 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="C224" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -4355,10 +4605,10 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="C225" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="226" spans="1:3">
@@ -4366,10 +4616,10 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="C226" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -4377,10 +4627,10 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="C227" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -4388,10 +4638,10 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="C228" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -4399,10 +4649,10 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="C229" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -4410,10 +4660,10 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="C230" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -4421,10 +4671,10 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="C231" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="232" spans="1:3">
@@ -4432,10 +4682,10 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="C232" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="233" spans="1:3">
@@ -4443,10 +4693,10 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="C233" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="234" spans="1:3">
@@ -4454,10 +4704,10 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="C234" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="235" spans="1:3">
@@ -4465,10 +4715,10 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C235" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="236" spans="1:3">
@@ -4476,10 +4726,10 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="C236" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="237" spans="1:3">
@@ -4487,10 +4737,10 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C237" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="238" spans="1:3">
@@ -4498,10 +4748,10 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="C238" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="239" spans="1:3">
@@ -4509,10 +4759,10 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="C239" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="240" spans="1:3">
@@ -4520,10 +4770,10 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="C240" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -4531,10 +4781,10 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="C241" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="1:3">
@@ -4542,10 +4792,10 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="C242" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -4553,10 +4803,10 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="C243" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="244" spans="1:3">
@@ -4564,10 +4814,10 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="C244" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -4575,10 +4825,10 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="C245" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="246" spans="1:3">
@@ -4586,10 +4836,10 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="C246" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="247" spans="1:3">
@@ -4597,10 +4847,10 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="C247" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="248" spans="1:3">
@@ -4608,10 +4858,10 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="C248" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="249" spans="1:3">
@@ -4619,10 +4869,10 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="C249" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="250" spans="1:3">
@@ -4630,10 +4880,10 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="C250" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -4641,10 +4891,10 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="C251" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -4652,10 +4902,10 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="C252" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -4663,10 +4913,10 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="C253" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -4674,10 +4924,10 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="C254" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -4685,10 +4935,10 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="C255" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="256" spans="1:3">
@@ -4696,10 +4946,10 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="C256" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="257" spans="1:3">
@@ -4707,10 +4957,10 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="C257" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="258" spans="1:3">
@@ -4718,10 +4968,10 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="C258" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="259" spans="1:3">
@@ -4729,10 +4979,10 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="C259" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="260" spans="1:3">
@@ -4740,10 +4990,10 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="C260" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="261" spans="1:3">
@@ -4751,10 +5001,10 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="C261" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4762,10 +5012,10 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="C262" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="263" spans="1:3">
@@ -4773,10 +5023,10 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="C263" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="264" spans="1:3">
@@ -4784,10 +5034,10 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="C264" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="265" spans="1:3">
@@ -4795,10 +5045,10 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="C265" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:3">
@@ -4806,10 +5056,10 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="C266" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="267" spans="1:3">
@@ -4817,10 +5067,10 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="C267" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -4828,10 +5078,10 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="C268" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="269" spans="1:3">
@@ -4839,10 +5089,10 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="C269" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="270" spans="1:3">
@@ -4850,10 +5100,10 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="C270" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="271" spans="1:3">
@@ -4861,10 +5111,10 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="C271" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correctly display ticker frequency.
</commit_message>
<xml_diff>
--- a/OptionTrades.xlsx
+++ b/OptionTrades.xlsx
@@ -1532,7 +1532,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Options!$F$2:$G$2</c:f>
+              <c:f>Options!$F$1:$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1546,7 +1546,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Options!$F$3:$G$3</c:f>
+              <c:f>Options!$F$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1626,21 +1626,78 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Options!$N$4:$O$4</c:f>
+              <c:f>Options!$O$2:$O$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>SPY</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>Ticker</c:v>
+                  <c:v>QQQ</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SQ</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AAPL</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>NVDA</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CHWY</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>TSLA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FSLY</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>VXX</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>BA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Options!$N$5:$O$14</c:f>
+              <c:f>Options!$P$2:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="0"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1678,13 +1735,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1708,13 +1765,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2035,6 +2092,18 @@
       <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1">
@@ -2046,11 +2115,23 @@
       <c r="C2" t="s">
         <v>284</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>468</v>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>197</v>
+      </c>
+      <c r="G2">
+        <v>73</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2063,14 +2144,14 @@
       <c r="C3" t="s">
         <v>285</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>197</v>
-      </c>
-      <c r="G3">
-        <v>73</v>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -2083,11 +2164,14 @@
       <c r="C4" t="s">
         <v>286</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>1</v>
+      <c r="N4" s="1">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2101,13 +2185,13 @@
         <v>287</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P5">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -2121,13 +2205,13 @@
         <v>288</v>
       </c>
       <c r="N6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P6">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -2141,13 +2225,13 @@
         <v>289</v>
       </c>
       <c r="N7" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P7">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -2161,13 +2245,13 @@
         <v>290</v>
       </c>
       <c r="N8" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P8">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2181,13 +2265,13 @@
         <v>291</v>
       </c>
       <c r="N9" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P9">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2201,13 +2285,13 @@
         <v>292</v>
       </c>
       <c r="N10" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="P10">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2221,13 +2305,13 @@
         <v>293</v>
       </c>
       <c r="N11" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P11">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2240,15 +2324,6 @@
       <c r="C12" t="s">
         <v>294</v>
       </c>
-      <c r="N12" s="1">
-        <v>7</v>
-      </c>
-      <c r="O12" t="s">
-        <v>9</v>
-      </c>
-      <c r="P12">
-        <v>10</v>
-      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1">
@@ -2260,15 +2335,6 @@
       <c r="C13" t="s">
         <v>295</v>
       </c>
-      <c r="N13" s="1">
-        <v>8</v>
-      </c>
-      <c r="O13" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13">
-        <v>10</v>
-      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1">
@@ -2279,15 +2345,6 @@
       </c>
       <c r="C14" t="s">
         <v>291</v>
-      </c>
-      <c r="N14" s="1">
-        <v>9</v>
-      </c>
-      <c r="O14" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14">
-        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:16">

</xml_diff>